<commit_message>
Updated write cells up to uipathauditorsdt for each row
</commit_message>
<xml_diff>
--- a/Steven(Schedule)/Schedule/Dummy QC Schedule Copy.xlsx
+++ b/Steven(Schedule)/Schedule/Dummy QC Schedule Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\UiPath\P3-schedulerassistant\Steven(Schedule)\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEBE208-4EB0-4D4D-8D4D-DF01C3D1DB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C89470-7CF3-4BC5-B6D0-89345BA2C6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4164" yWindow="2136" windowWidth="15972" windowHeight="9768" tabRatio="605" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="340">
   <si>
     <t>Rules:</t>
   </si>
@@ -13492,10 +13492,25 @@
         <f>D4*E4</f>
         <v>39</v>
       </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
       <c r="I4">
         <f>6+1</f>
         <v>7</v>
       </c>
+      <c r="J4" t="s">
+        <v>338</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="M4" t="s">
         <v>333</v>
       </c>
@@ -13572,10 +13587,25 @@
         <f>D6*E6</f>
         <v>42</v>
       </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
       <c r="I6">
         <f>5+1</f>
         <v>6</v>
       </c>
+      <c r="J6" t="s">
+        <v>338</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M6" t="s">
         <v>334</v>
       </c>
@@ -13913,10 +13943,25 @@
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
       <c r="I17">
         <f>8+1</f>
         <v>9</v>
       </c>
+      <c r="J17" t="s">
+        <v>338</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="M17" t="s">
         <v>334</v>
       </c>
@@ -13950,6 +13995,9 @@
       <c r="G18" t="s">
         <v>35</v>
       </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
       <c r="I18">
         <f>4+1</f>
         <v>5</v>
@@ -14027,10 +14075,25 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>46</v>
+      </c>
       <c r="I20">
         <f>3+1</f>
         <v>4</v>
       </c>
+      <c r="J20" t="s">
+        <v>337</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="M20" t="s">
         <v>335</v>
       </c>
@@ -14061,10 +14124,22 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
       <c r="I21">
         <f>0+1</f>
         <v>1</v>
       </c>
+      <c r="J21" t="s">
+        <v>338</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.5</v>
+      </c>
       <c r="M21" t="s">
         <v>334</v>
       </c>
@@ -14559,11 +14634,11 @@
       </c>
       <c r="D37">
         <f>COUNTIF($G$1:G$34,C37)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <f>AVERAGEIF($G$3:$G$35,C37,$I$3:$I$35)</f>
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="F37">
         <f>SUMIF($G$3:$G$34, C37, $D$3:$D$34)</f>
@@ -14571,7 +14646,7 @@
       </c>
       <c r="G37">
         <f>SUMIF($G$3:$G$31, C37, $F$3:$F$31)</f>
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="O37" t="s">
         <v>157</v>
@@ -14590,11 +14665,11 @@
       </c>
       <c r="D38">
         <f>COUNTIF($G$1:G$34,C38)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E38">
         <f>AVERAGEIF($G$3:$G$34,C38,$I$3:$I$34)</f>
-        <v>5</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="F38">
         <f>SUMIF($G$3:$G$34, C38, $D$3:$D$34)</f>
@@ -14602,7 +14677,7 @@
       </c>
       <c r="G38">
         <f>SUMIF($G$3:$G$31, C38, $F$3:$F$31)</f>
-        <v>54</v>
+        <v>157.5</v>
       </c>
       <c r="O38" t="s">
         <v>159</v>
@@ -14714,7 +14789,7 @@
       </c>
       <c r="D42">
         <f>SUM(D37:D40)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <f>SUM(F37:F40)</f>
@@ -14722,7 +14797,7 @@
       </c>
       <c r="G42">
         <f>SUM(G37:G40)</f>
-        <v>135</v>
+        <v>319.5</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -14731,7 +14806,7 @@
       </c>
       <c r="D43">
         <f>D42/COUNTA(C37:C40)</f>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="F43">
         <f>F42/COUNTA(C37:C40)</f>
@@ -14739,7 +14814,7 @@
       </c>
       <c r="G43">
         <f>G42/COUNTA(C37:C40)</f>
-        <v>33.75</v>
+        <v>79.875</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -15170,21 +15245,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035320A12CFF460459638DE9B86DD9357" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f11676696cc246df58d12072c86cf252">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5789d6d3-4852-43c5-9082-41a0df76b368" xmlns:ns4="f28bebd9-3202-45a0-b989-5e5ae93a89b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ea6d730d764c2aef8b02e40be4db643" ns3:_="" ns4:_="">
     <xsd:import namespace="5789d6d3-4852-43c5-9082-41a0df76b368"/>
@@ -15407,6 +15467,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C43A65-5EE1-4708-A032-9E6F3F603D25}">
   <ds:schemaRefs>
@@ -15416,23 +15491,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F62D5D-402C-4D37-8B1B-B293D3FE1710}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E74CAD0-3F93-445C-B91B-678382B98543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15449,4 +15507,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F62D5D-402C-4D37-8B1B-B293D3FE1710}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>